<commit_message>
Started using load_factor_scenarios in ipynb instead of manual uploading and modification
</commit_message>
<xml_diff>
--- a/Data/data.xlsx
+++ b/Data/data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Ilmari/Documents/OR semma/entropy-poolin/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Ilmari/Documents/OR semma/entropy-poolin/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C01CCBFB-3086-424F-A340-E15D89F3C2FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50F547B9-9E1F-0E42-A667-A43D9E19F879}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15900" activeTab="1" xr2:uid="{F9C29C47-E65C-40D9-8125-D2F4D60475BD}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15900" xr2:uid="{F9C29C47-E65C-40D9-8125-D2F4D60475BD}"/>
   </bookViews>
   <sheets>
     <sheet name="DATA" sheetId="3" r:id="rId1"/>
@@ -1894,7 +1894,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BAF92571-C8FA-4993-8EF6-2CFE52B24ECF}">
   <dimension ref="A1:AL253"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="S14" sqref="S14"/>
     </sheetView>
   </sheetViews>
@@ -30784,7 +30784,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A557845-7B97-49DA-9E9C-9E1E004351D8}">
   <dimension ref="A1:D37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>

</xml_diff>